<commit_message>
Se completo la prueba de la capa Batchnorm en Python, se deja ipynb
</commit_message>
<xml_diff>
--- a/PythonImplementations/BatchNormalization/EntendiendoBN.xlsx
+++ b/PythonImplementations/BatchNormalization/EntendiendoBN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Embedded_AI\ImplementacionCapas\LayersImplementationsCNN\PythonImplementations\BatchNormalization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AD50F6F-6233-49AC-8549-A27302B8BD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A2B412-7462-4DD4-99BE-945262EB5EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="14640" windowHeight="13455" xr2:uid="{E907E16A-777B-4A63-B53D-C1F88FE012E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13455" xr2:uid="{E907E16A-777B-4A63-B53D-C1F88FE012E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Voltaje X</t>
   </si>
@@ -49,12 +49,27 @@
   </si>
   <si>
     <t>Epsilon</t>
+  </si>
+  <si>
+    <t>VAR</t>
+  </si>
+  <si>
+    <t>Norma 1</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>Beta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,9 +114,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,156 +432,265 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64651440-1B3A-43A4-9CB1-E7E49E20E1AB}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="B2:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E13" sqref="D13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="1">
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <f>(B2-$B$14)/(SQRT($B$15+$B$16))</f>
-        <v>-1.5811385138565184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
+      <c r="D3" s="1">
+        <f>(C3-$C$15)/(SQRT($C$16+$C$17))</f>
+        <v>-1.5811388300841895</v>
+      </c>
+      <c r="F3" s="2">
+        <f>$C$19*(C3-$C$15)/(SQRT($C$16+$C$17))+$C$20</f>
+        <v>-0.76990654405048331</v>
+      </c>
+      <c r="H3" s="1">
+        <f>(C3-$C$15)^2</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="1">
         <v>1.5</v>
       </c>
-      <c r="C3" s="1">
-        <f t="shared" ref="C3:C12" si="0">(B3-$B$14)/(SQRT($B$15+$B$16))</f>
-        <v>-1.2649108110852147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="1">
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D13" si="0">(C4-$C$15)/(SQRT($C$16+$C$17))</f>
+        <v>-1.2649110640673518</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" ref="F4:F13" si="1">$C$19*(C4-$C$15)/(SQRT($C$16+$C$17))+$C$20</f>
+        <v>-0.56173652524038653</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H13" si="2">(C4-$C$15)^2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.94868310831391101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.94868329805051377</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.35356650643028992</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="2"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
         <v>2.5</v>
       </c>
-      <c r="C5" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.63245540554260737</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.63245553203367588</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.1453964876201933</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="1">
         <v>3</v>
       </c>
-      <c r="C6" s="1">
-        <f t="shared" si="0"/>
-        <v>-0.31622770277130369</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.31622776601683794</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="1"/>
+        <v>6.2773531189903337E-2</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
         <v>3.5</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D8" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27094354999999998</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
         <v>4</v>
       </c>
-      <c r="C8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.31622770277130369</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.31622776601683794</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.47911356881009659</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
         <v>4.5</v>
       </c>
-      <c r="C9" s="1">
-        <f t="shared" si="0"/>
-        <v>0.63245540554260737</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.63245553203367588</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.68728358762019326</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="1">
         <v>5</v>
       </c>
-      <c r="C10" s="1">
-        <f t="shared" si="0"/>
-        <v>0.94868310831391101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.94868329805051377</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.89545360643028982</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="2"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="1">
         <v>5.5</v>
       </c>
-      <c r="C11" s="1">
-        <f t="shared" si="0"/>
-        <v>1.2649108110852147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2649110640673518</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1036236252403866</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="1">
         <v>6</v>
       </c>
-      <c r="C12" s="1">
-        <f t="shared" si="0"/>
-        <v>1.5811385138565184</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5811388300841895</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3117936440504832</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="2"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="1">
+        <f>SUM(H3:H13)/11</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B14">
-        <f>AVERAGE(B2:B12)</f>
+      <c r="C15" s="1">
+        <f>AVERAGE(C3:C13)</f>
         <v>3.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B15">
+      <c r="C16" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B16">
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>0.20645763</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>0.65829139999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>0.27094354999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>